<commit_message>
Added power sequencing for ADC. Split IMU into 2 boards.
</commit_message>
<xml_diff>
--- a/electrical/imu/imu_power_estimate.xlsx
+++ b/electrical/imu/imu_power_estimate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>ADXL325</t>
   </si>
@@ -39,9 +39,6 @@
     <t>OPA350</t>
   </si>
   <si>
-    <t>LM1117DT-1.8</t>
-  </si>
-  <si>
     <t>HMC1053</t>
   </si>
   <si>
@@ -73,6 +70,21 @@
   </si>
   <si>
     <t>TOTAL 3.3V Current:</t>
+  </si>
+  <si>
+    <t>ANALOG BOARD 3.3V Current</t>
+  </si>
+  <si>
+    <t>ANALOG BOARD 5V Current</t>
+  </si>
+  <si>
+    <t>DIGITAL BOARD 3.3V Current</t>
+  </si>
+  <si>
+    <t>DIGITAL BOARD 5V Current</t>
+  </si>
+  <si>
+    <t>TPS-1.8</t>
   </si>
 </sst>
 </file>
@@ -413,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -434,22 +446,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -489,18 +501,18 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D7" si="0">B3*C3</f>
         <v>22.5</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="1">B3*E3</f>
+        <f t="shared" ref="F3:F7" si="1">B3*E3</f>
         <v>13.5</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="2">D3*E3</f>
+        <f t="shared" ref="G3:G7" si="2">D3*E3</f>
         <v>67.5</v>
       </c>
     </row>
@@ -559,33 +571,33 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>14</v>
@@ -611,7 +623,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>3.5000000000000003E-2</v>
@@ -637,7 +649,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <f>3.3/200*1000 + 10</f>
@@ -664,7 +676,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0.13</v>
@@ -690,7 +702,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <f>114-3-2-2-2-2-1-3-2.5-1.5</f>
@@ -717,25 +729,25 @@
     </row>
     <row r="15" spans="1:7">
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <f>SUM(F3+F4+F5+F6+F7)</f>
-        <v>47.3</v>
+        <v>62.3</v>
       </c>
       <c r="C16">
         <f>B16*5</f>
-        <v>236.5</v>
+        <v>311.5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <f>SUM(F2+F8+F9+F10+F11)</f>
@@ -744,6 +756,41 @@
       <c r="C17">
         <f>B17*3.3</f>
         <v>402.64949999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <f>SUM(F2,F8,F6)</f>
+        <v>20.385000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <f>SUM(F5,F4,F3,F7)</f>
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <f>SUM(F11,F10,F9)</f>
+        <v>121.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the IMU controller PCB (IMU_CPU.1) and renamed the projects imu_cpu and imu_sense.
</commit_message>
<xml_diff>
--- a/electrical/imu/imu_power_estimate.xlsx
+++ b/electrical/imu/imu_power_estimate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>ADXL325</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>TPS-1.8</t>
+  </si>
+  <si>
+    <t>ANALOG BOARD 1.8V current</t>
+  </si>
+  <si>
+    <t>MCP1791T-5002E/DCCT-ND</t>
+  </si>
+  <si>
+    <t>Max current 70mA, max power at 120 degrees F is 1.22 Watts, we are dissipating &lt; .6W</t>
   </si>
 </sst>
 </file>
@@ -425,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -436,7 +445,8 @@
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -558,15 +568,15 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>5.2</v>
+        <v>10.4</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -738,14 +748,14 @@
       </c>
       <c r="B16">
         <f>SUM(F3+F4+F5+F6+F7)</f>
-        <v>62.3</v>
+        <v>67.5</v>
       </c>
       <c r="C16">
         <f>B16*5</f>
-        <v>311.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>337.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -758,38 +768,52 @@
         <v>402.64949999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21">
-        <f>SUM(F2,F8,F6)</f>
-        <v>20.385000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <f>SUM(F2,F8)</f>
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22">
         <f>SUM(F5,F4,F3,F7)</f>
-        <v>42.3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+        <v>47.5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f>SUM(F11,F10,F9)</f>
         <v>121.63</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>0</v>
       </c>
     </row>

</xml_diff>